<commit_message>
Update Contribution Document (2).xlsx
Update contribution info
</commit_message>
<xml_diff>
--- a/Contribution Document (2).xlsx
+++ b/Contribution Document (2).xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamud\AndroidStudioProjects\prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4706356770a3a103/Desktop/test/W23_G1_GTPredict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E22A11-CCE5-4250-B57F-7A136FA1439C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{68E22A11-CCE5-4250-B57F-7A136FA1439C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4ED9B8-1447-412D-96C4-8D00E2B65953}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EDEFFC3-B721-47BD-951B-C9BDD1B29C16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{6EDEFFC3-B721-47BD-951B-C9BDD1B29C16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>Week2</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Line Chart extention</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GITHUB issues and update with bug fix on text color </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding splash activity and logos, icon for app but two icon shows not sure why have to check </t>
   </si>
 </sst>
 </file>
@@ -279,7 +288,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,6 +311,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -637,21 +648,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558BB9C9-9A0D-4E25-BAC3-4371389C6F28}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="5" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -665,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -679,7 +692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -693,7 +706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -708,7 +721,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -716,7 +729,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -724,7 +737,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -738,7 +751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -746,7 +759,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -754,15 +767,21 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="18">
+        <v>44990</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -770,7 +789,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -778,7 +797,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -786,15 +805,21 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="19">
+        <v>44999</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -802,7 +827,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -810,7 +835,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -818,7 +843,7 @@
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>1</v>
       </c>
@@ -826,7 +851,7 @@
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
@@ -834,7 +859,7 @@
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>3</v>
       </c>
@@ -842,7 +867,7 @@
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>7</v>
       </c>
@@ -850,7 +875,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>1</v>
       </c>
@@ -858,7 +883,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>2</v>
       </c>
@@ -866,7 +891,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>3</v>
       </c>
@@ -874,7 +899,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>12</v>
       </c>
@@ -882,7 +907,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>1</v>
       </c>
@@ -890,7 +915,7 @@
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>2</v>
       </c>
@@ -898,7 +923,7 @@
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>3</v>
       </c>
@@ -906,7 +931,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>11</v>
       </c>
@@ -914,7 +939,7 @@
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>1</v>
       </c>
@@ -922,7 +947,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>2</v>
       </c>
@@ -930,7 +955,7 @@
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>3</v>
       </c>
@@ -938,7 +963,7 @@
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>10</v>
       </c>
@@ -946,7 +971,7 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>1</v>
       </c>
@@ -954,7 +979,7 @@
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>2</v>
       </c>
@@ -962,7 +987,7 @@
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>3</v>
       </c>
@@ -970,7 +995,7 @@
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1003,7 @@
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>1</v>
       </c>
@@ -986,7 +1011,7 @@
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1019,7 @@
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>3</v>
       </c>
@@ -1002,7 +1027,7 @@
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1035,7 @@
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1043,7 @@
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1051,7 @@
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>3</v>
       </c>

</xml_diff>